<commit_message>
Updated capital structure database
</commit_message>
<xml_diff>
--- a/teaching/traditional_assets/database/data/anguilla/anguilla_entertainment.xlsx
+++ b/teaching/traditional_assets/database/data/anguilla/anguilla_entertainment.xlsx
@@ -590,23 +590,26 @@
           <t>Entertainment</t>
         </is>
       </c>
+      <c r="D2">
+        <v>1.726</v>
+      </c>
       <c r="G2">
-        <v>-0.6887966804979253</v>
+        <v>-0.04166666666666666</v>
       </c>
       <c r="H2">
-        <v>-1.112033195020747</v>
+        <v>-0.2274305555555556</v>
       </c>
       <c r="I2">
-        <v>-0.6932743209250716</v>
+        <v>-0.1499473603888499</v>
       </c>
       <c r="J2">
-        <v>-0.6932743209250716</v>
+        <v>-0.1499473603888499</v>
       </c>
       <c r="K2">
-        <v>-1.65</v>
+        <v>-14</v>
       </c>
       <c r="L2">
-        <v>-0.6846473029045642</v>
+        <v>-2.430555555555556</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -630,70 +633,70 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0.8120000000000001</v>
+        <v>1.14</v>
       </c>
       <c r="V2">
-        <v>0.03171875</v>
+        <v>0.02024866785079929</v>
       </c>
       <c r="W2">
-        <v>-1.571428571428571</v>
+        <v>-0.6422018348623852</v>
       </c>
       <c r="X2">
-        <v>0.1445553831000524</v>
+        <v>0.09330194337382679</v>
       </c>
       <c r="Y2">
-        <v>-1.715983954528624</v>
+        <v>-0.735503778236212</v>
       </c>
       <c r="Z2">
-        <v>11.26402099340051</v>
+        <v>0.2704671816073499</v>
       </c>
       <c r="AA2">
-        <v>-7.809056505085485</v>
+        <v>-0.0405558399538338</v>
       </c>
       <c r="AB2">
-        <v>0.1436736792283541</v>
+        <v>0.09304293101393067</v>
       </c>
       <c r="AC2">
-        <v>-7.95273018431384</v>
+        <v>-0.1335987709677645</v>
       </c>
       <c r="AD2">
-        <v>0.119</v>
+        <v>0.03</v>
       </c>
       <c r="AE2">
-        <v>0.1639555671471137</v>
+        <v>0.3084839791988757</v>
       </c>
       <c r="AF2">
-        <v>0.2829555671471137</v>
+        <v>0.3384839791988756</v>
       </c>
       <c r="AG2">
-        <v>-0.5290444328528864</v>
+        <v>-0.8015160208011243</v>
       </c>
       <c r="AH2">
-        <v>0.01093211964966881</v>
+        <v>0.005976218913683984</v>
       </c>
       <c r="AI2">
-        <v>0.01281330147528203</v>
+        <v>0.04138712994483752</v>
       </c>
       <c r="AJ2">
-        <v>-0.02110188546407638</v>
+        <v>-0.0144421246011249</v>
       </c>
       <c r="AK2">
-        <v>-0.02487168153695891</v>
+        <v>-0.1138762300475327</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>-0.004</v>
+        <v>-0.002</v>
       </c>
       <c r="AN2">
-        <v>-0.07354758961681088</v>
+        <v>-0.1260504201680672</v>
       </c>
       <c r="AP2">
-        <v>0.3269743095506096</v>
+        <v>3.367714373113967</v>
       </c>
       <c r="AQ2">
-        <v>417.5</v>
+        <v>452.5</v>
       </c>
     </row>
     <row r="3">
@@ -712,23 +715,26 @@
           <t>Entertainment</t>
         </is>
       </c>
+      <c r="D3">
+        <v>1.726</v>
+      </c>
       <c r="G3">
-        <v>-0.6887966804979253</v>
+        <v>-0.04166666666666666</v>
       </c>
       <c r="H3">
-        <v>-1.112033195020747</v>
+        <v>-0.2274305555555556</v>
       </c>
       <c r="I3">
-        <v>-0.6932743209250716</v>
+        <v>-0.1499473603888499</v>
       </c>
       <c r="J3">
-        <v>-0.6932743209250716</v>
+        <v>-0.1499473603888499</v>
       </c>
       <c r="K3">
-        <v>-1.65</v>
+        <v>-14</v>
       </c>
       <c r="L3">
-        <v>-0.6846473029045642</v>
+        <v>-2.430555555555556</v>
       </c>
       <c r="M3">
         <v>-0</v>
@@ -752,70 +758,70 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0.8120000000000001</v>
+        <v>1.14</v>
       </c>
       <c r="V3">
-        <v>0.03171875</v>
+        <v>0.02024866785079929</v>
       </c>
       <c r="W3">
-        <v>-1.571428571428571</v>
+        <v>-0.6422018348623852</v>
       </c>
       <c r="X3">
-        <v>0.1445553831000524</v>
+        <v>0.09330194337382679</v>
       </c>
       <c r="Y3">
-        <v>-1.715983954528624</v>
+        <v>-0.735503778236212</v>
       </c>
       <c r="Z3">
-        <v>11.26402099340051</v>
+        <v>0.2704671816073499</v>
       </c>
       <c r="AA3">
-        <v>-7.809056505085485</v>
+        <v>-0.0405558399538338</v>
       </c>
       <c r="AB3">
-        <v>0.1436736792283541</v>
+        <v>0.09304293101393067</v>
       </c>
       <c r="AC3">
-        <v>-7.95273018431384</v>
+        <v>-0.1335987709677645</v>
       </c>
       <c r="AD3">
-        <v>0.119</v>
+        <v>0.03</v>
       </c>
       <c r="AE3">
-        <v>0.1639555671471137</v>
+        <v>0.3084839791988757</v>
       </c>
       <c r="AF3">
-        <v>0.2829555671471137</v>
+        <v>0.3384839791988756</v>
       </c>
       <c r="AG3">
-        <v>-0.5290444328528864</v>
+        <v>-0.8015160208011243</v>
       </c>
       <c r="AH3">
-        <v>0.01093211964966881</v>
+        <v>0.005976218913683984</v>
       </c>
       <c r="AI3">
-        <v>0.01281330147528203</v>
+        <v>0.04138712994483752</v>
       </c>
       <c r="AJ3">
-        <v>-0.02110188546407638</v>
+        <v>-0.0144421246011249</v>
       </c>
       <c r="AK3">
-        <v>-0.02487168153695891</v>
+        <v>-0.1138762300475327</v>
       </c>
       <c r="AL3">
         <v>0</v>
       </c>
       <c r="AM3">
-        <v>-0.004</v>
+        <v>-0.002</v>
       </c>
       <c r="AN3">
-        <v>-0.07354758961681088</v>
+        <v>-0.1260504201680672</v>
       </c>
       <c r="AP3">
-        <v>0.3269743095506096</v>
+        <v>3.367714373113967</v>
       </c>
       <c r="AQ3">
-        <v>417.5</v>
+        <v>452.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>